<commit_message>
added key for july 14
</commit_message>
<xml_diff>
--- a/data-raw/Growth curve well labels.xlsx
+++ b/data-raw/Growth curve well labels.xlsx
@@ -1,58 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sveta\Documents\B Lab\cross-tolerance\data-raw\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF497E23-F5D2-4C62-8D44-7CC9FDEF5295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
-    <sheet name="16.06, 20.06" sheetId="1" r:id="rId1"/>
-    <sheet name="joey-edit-16.06, 20.06" sheetId="2" r:id="rId2"/>
-    <sheet name="24.06" sheetId="3" r:id="rId3"/>
-    <sheet name="28.06, 30 and 34 deg" sheetId="4" r:id="rId4"/>
-    <sheet name="29.06, 37 deg" sheetId="5" r:id="rId5"/>
-    <sheet name="30.06, 40 and 41 deg" sheetId="6" r:id="rId6"/>
-    <sheet name="01.07, 25 deg" sheetId="7" r:id="rId7"/>
-    <sheet name="04.07, 18 deg" sheetId="8" r:id="rId8"/>
-    <sheet name="05.07, 30 deg" sheetId="9" r:id="rId9"/>
-    <sheet name="05.07, 40 deg" sheetId="10" r:id="rId10"/>
-    <sheet name="06.07, 37 deg" sheetId="11" r:id="rId11"/>
-    <sheet name="06.07, 40.5 deg" sheetId="12" r:id="rId12"/>
-    <sheet name="11.07, 41 deg" sheetId="13" r:id="rId13"/>
+    <sheet state="visible" name="16.06, 20.06" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="joey-edit-16.06, 20.06" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="24.06" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="28.06, 30 and 34 deg" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="29.06, 37 deg" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="30.06, 40 and 41 deg" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="01.07, 25 deg" sheetId="7" r:id="rId10"/>
+    <sheet state="visible" name="04.07, 18 deg" sheetId="8" r:id="rId11"/>
+    <sheet state="visible" name="05.07, 30 deg" sheetId="9" r:id="rId12"/>
+    <sheet state="visible" name="05.07, 40 deg" sheetId="10" r:id="rId13"/>
+    <sheet state="visible" name="06.07, 37 deg" sheetId="11" r:id="rId14"/>
+    <sheet state="visible" name="06.07, 40.5 deg" sheetId="12" r:id="rId15"/>
+    <sheet state="visible" name="11.07, 41 deg" sheetId="13" r:id="rId16"/>
+    <sheet state="visible" name="14.07, 30 deg" sheetId="14" r:id="rId17"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
+    <comment authorId="0" ref="A1">
       <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>randomized
+        <t xml:space="preserve">randomized
 Only 8 replicates were done for fRS585
 25*C
 Blank (Yellow) - A2, F3, D4, G5, B8, E9, G9, C10
 Culture (Green)- G2, C3, B5, E6, G7, D8, B10, F11
 	-Sveta U</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -60,26 +44,18 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000001000000}">
+    <comment authorId="0" ref="A1">
       <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>randomized!
+        <t xml:space="preserve">randomized!
 30 deg C:
 purple = blank, B7, B10, C3, D11, E6, F2, F9, G5
 blue = strain, B5, D2, D7, D9, E4, G3, G7, G11
 	-Sveta U</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -87,25 +63,17 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0900-000001000000}">
+    <comment authorId="0" ref="A1">
       <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>40 deg C:
+        <t xml:space="preserve">40 deg C:
 red = blank, B5, B7, B11, C2, E4, E9, F7, G11
 yellow = strain, B3, C9, D3, D6, E11, F2, G4, G9
 	-Sveta U</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -113,25 +81,17 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0A00-000001000000}">
+    <comment authorId="0" ref="A1">
       <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>37*C
+        <t xml:space="preserve">37*C
 Blank (Green) - C2, F3, G5, E6, B8, F8, D10, G10
 Culture (Red) - G2, D3, B4, D7, G7, C9, B11, E11
 	-Sveta U</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -139,25 +99,17 @@
 </file>
 
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0B00-000001000000}">
+    <comment authorId="0" ref="A1">
       <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>40.5*C
+        <t xml:space="preserve">40.5*C
 Blank (blue) - F2, D4, F6, B8, C9, D10, G11, G8
 Culture (Purple) - D2, G4, C5, E5, E8, F10, B10, D11
 	-Sveta U</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -165,26 +117,35 @@
 </file>
 
 <file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0C00-000001000000}">
+    <comment authorId="0" ref="A1">
       <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>Randomized wells
+        <t xml:space="preserve">Randomized wells
 41*C
 Blank (yellow): G2, C4, F4, E6, B7, C9, F10, D11
 Culture (blue): D3, B4, G4, G7, D8, F9, B10, G11
 	-Sveta U</t>
-        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="A1">
+      <text>
+        <t xml:space="preserve">Blank (green) - C3, G4, D5, F6, C8, B10, F10, D11
+Culture (purple) - D2, F3, C4, D6, B7, E8, G9, C10
+	-Ijeoma Nwafor</t>
       </text>
     </comment>
   </commentList>
@@ -192,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="123">
   <si>
     <t xml:space="preserve">well </t>
   </si>
@@ -566,33 +527,31 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fonts count="5">
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Georgia"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Georgia"/>
     </font>
@@ -602,46 +561,101 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+  <cellXfs count="7">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -831,23 +845,20 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F97"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -855,7 +866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -863,7 +874,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -871,7 +882,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -879,7 +890,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -887,9 +898,9 @@
         <v>3</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -897,9 +908,9 @@
         <v>3</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -907,9 +918,9 @@
         <v>3</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -917,9 +928,9 @@
         <v>3</v>
       </c>
       <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -927,9 +938,9 @@
         <v>3</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -937,9 +948,9 @@
         <v>3</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -947,9 +958,9 @@
         <v>3</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -957,9 +968,9 @@
         <v>3</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -967,103 +978,103 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26">
       <c r="A26" s="1" t="s">
         <v>28</v>
       </c>
@@ -1071,7 +1082,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27">
       <c r="A27" s="1" t="s">
         <v>30</v>
       </c>
@@ -1079,7 +1090,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28">
       <c r="A28" s="1" t="s">
         <v>31</v>
       </c>
@@ -1087,7 +1098,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29">
       <c r="A29" s="1" t="s">
         <v>32</v>
       </c>
@@ -1095,7 +1106,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30">
       <c r="A30" s="1" t="s">
         <v>33</v>
       </c>
@@ -1103,7 +1114,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31">
       <c r="A31" s="1" t="s">
         <v>34</v>
       </c>
@@ -1111,7 +1122,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32">
       <c r="A32" s="1" t="s">
         <v>35</v>
       </c>
@@ -1119,7 +1130,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33">
       <c r="A33" s="1" t="s">
         <v>36</v>
       </c>
@@ -1127,7 +1138,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34">
       <c r="A34" s="1" t="s">
         <v>37</v>
       </c>
@@ -1135,7 +1146,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35">
       <c r="A35" s="1" t="s">
         <v>38</v>
       </c>
@@ -1143,7 +1154,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36">
       <c r="A36" s="1" t="s">
         <v>39</v>
       </c>
@@ -1151,7 +1162,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37">
       <c r="A37" s="1" t="s">
         <v>40</v>
       </c>
@@ -1159,7 +1170,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38">
       <c r="A38" s="1" t="s">
         <v>41</v>
       </c>
@@ -1167,7 +1178,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39">
       <c r="A39" s="1" t="s">
         <v>43</v>
       </c>
@@ -1175,7 +1186,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40">
       <c r="A40" s="1" t="s">
         <v>44</v>
       </c>
@@ -1183,7 +1194,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41">
       <c r="A41" s="1" t="s">
         <v>45</v>
       </c>
@@ -1191,7 +1202,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42">
       <c r="A42" s="1" t="s">
         <v>46</v>
       </c>
@@ -1199,7 +1210,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43">
       <c r="A43" s="1" t="s">
         <v>47</v>
       </c>
@@ -1207,7 +1218,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44">
       <c r="A44" s="1" t="s">
         <v>48</v>
       </c>
@@ -1215,7 +1226,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45">
       <c r="A45" s="1" t="s">
         <v>49</v>
       </c>
@@ -1223,7 +1234,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46">
       <c r="A46" s="1" t="s">
         <v>50</v>
       </c>
@@ -1231,7 +1242,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47">
       <c r="A47" s="1" t="s">
         <v>51</v>
       </c>
@@ -1239,7 +1250,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48">
       <c r="A48" s="1" t="s">
         <v>52</v>
       </c>
@@ -1247,7 +1258,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49">
       <c r="A49" s="1" t="s">
         <v>53</v>
       </c>
@@ -1255,7 +1266,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50">
       <c r="A50" s="1" t="s">
         <v>54</v>
       </c>
@@ -1263,7 +1274,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51">
       <c r="A51" s="1" t="s">
         <v>56</v>
       </c>
@@ -1271,7 +1282,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52">
       <c r="A52" s="1" t="s">
         <v>57</v>
       </c>
@@ -1279,7 +1290,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53">
       <c r="A53" s="1" t="s">
         <v>58</v>
       </c>
@@ -1287,7 +1298,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54">
       <c r="A54" s="1" t="s">
         <v>59</v>
       </c>
@@ -1295,7 +1306,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55">
       <c r="A55" s="1" t="s">
         <v>60</v>
       </c>
@@ -1303,7 +1314,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56">
       <c r="A56" s="1" t="s">
         <v>61</v>
       </c>
@@ -1311,7 +1322,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57">
       <c r="A57" s="1" t="s">
         <v>62</v>
       </c>
@@ -1319,7 +1330,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="58">
       <c r="A58" s="1" t="s">
         <v>63</v>
       </c>
@@ -1327,7 +1338,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59">
       <c r="A59" s="1" t="s">
         <v>64</v>
       </c>
@@ -1335,7 +1346,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60">
       <c r="A60" s="1" t="s">
         <v>65</v>
       </c>
@@ -1343,7 +1354,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="61">
       <c r="A61" s="1" t="s">
         <v>66</v>
       </c>
@@ -1351,7 +1362,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="62">
       <c r="A62" s="1" t="s">
         <v>67</v>
       </c>
@@ -1359,7 +1370,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="63">
       <c r="A63" s="1" t="s">
         <v>69</v>
       </c>
@@ -1367,7 +1378,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="64">
       <c r="A64" s="1" t="s">
         <v>70</v>
       </c>
@@ -1375,7 +1386,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="65">
       <c r="A65" s="1" t="s">
         <v>71</v>
       </c>
@@ -1383,7 +1394,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="66">
       <c r="A66" s="1" t="s">
         <v>72</v>
       </c>
@@ -1391,7 +1402,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="67">
       <c r="A67" s="1" t="s">
         <v>73</v>
       </c>
@@ -1399,7 +1410,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="68">
       <c r="A68" s="1" t="s">
         <v>74</v>
       </c>
@@ -1407,7 +1418,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="69">
       <c r="A69" s="1" t="s">
         <v>75</v>
       </c>
@@ -1415,7 +1426,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="70">
       <c r="A70" s="1" t="s">
         <v>76</v>
       </c>
@@ -1423,7 +1434,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="71">
       <c r="A71" s="1" t="s">
         <v>77</v>
       </c>
@@ -1431,7 +1442,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="72">
       <c r="A72" s="1" t="s">
         <v>78</v>
       </c>
@@ -1439,7 +1450,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="73">
       <c r="A73" s="1" t="s">
         <v>79</v>
       </c>
@@ -1447,7 +1458,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="74">
       <c r="A74" s="1" t="s">
         <v>80</v>
       </c>
@@ -1455,7 +1466,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="75">
       <c r="A75" s="1" t="s">
         <v>82</v>
       </c>
@@ -1463,7 +1474,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="76">
       <c r="A76" s="1" t="s">
         <v>83</v>
       </c>
@@ -1471,7 +1482,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="77">
       <c r="A77" s="1" t="s">
         <v>84</v>
       </c>
@@ -1479,7 +1490,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="78">
       <c r="A78" s="1" t="s">
         <v>85</v>
       </c>
@@ -1487,7 +1498,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="79">
       <c r="A79" s="1" t="s">
         <v>86</v>
       </c>
@@ -1495,7 +1506,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="80">
       <c r="A80" s="1" t="s">
         <v>87</v>
       </c>
@@ -1503,7 +1514,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81">
       <c r="A81" s="1" t="s">
         <v>88</v>
       </c>
@@ -1511,7 +1522,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="82">
       <c r="A82" s="1" t="s">
         <v>89</v>
       </c>
@@ -1519,7 +1530,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="83">
       <c r="A83" s="1" t="s">
         <v>90</v>
       </c>
@@ -1527,7 +1538,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="84">
       <c r="A84" s="1" t="s">
         <v>91</v>
       </c>
@@ -1535,7 +1546,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="85">
       <c r="A85" s="1" t="s">
         <v>92</v>
       </c>
@@ -1543,7 +1554,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="86">
       <c r="A86" s="1" t="s">
         <v>93</v>
       </c>
@@ -1551,7 +1562,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="87">
       <c r="A87" s="1" t="s">
         <v>95</v>
       </c>
@@ -1559,7 +1570,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="88">
       <c r="A88" s="1" t="s">
         <v>96</v>
       </c>
@@ -1567,7 +1578,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="89">
       <c r="A89" s="1" t="s">
         <v>97</v>
       </c>
@@ -1575,7 +1586,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="90">
       <c r="A90" s="1" t="s">
         <v>99</v>
       </c>
@@ -1583,7 +1594,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="91">
       <c r="A91" s="1" t="s">
         <v>100</v>
       </c>
@@ -1591,7 +1602,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="92">
       <c r="A92" s="1" t="s">
         <v>101</v>
       </c>
@@ -1599,7 +1610,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="93">
       <c r="A93" s="1" t="s">
         <v>102</v>
       </c>
@@ -1607,7 +1618,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="94">
       <c r="A94" s="1" t="s">
         <v>103</v>
       </c>
@@ -1615,7 +1626,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="95">
       <c r="A95" s="1" t="s">
         <v>104</v>
       </c>
@@ -1623,7 +1634,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="96">
       <c r="A96" s="1" t="s">
         <v>105</v>
       </c>
@@ -1631,7 +1642,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97">
       <c r="A97" s="1" t="s">
         <v>106</v>
       </c>
@@ -1640,22 +1651,21 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>107</v>
       </c>
@@ -1663,7 +1673,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -1671,7 +1681,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" s="1" t="s">
         <v>37</v>
       </c>
@@ -1679,7 +1689,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" s="1" t="s">
         <v>44</v>
       </c>
@@ -1687,7 +1697,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="A5" s="1" t="s">
         <v>47</v>
       </c>
@@ -1695,34 +1705,34 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="A6" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7">
       <c r="A7" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8">
       <c r="A8" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9">
       <c r="A9" s="1" t="s">
         <v>89</v>
       </c>
@@ -1730,7 +1740,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -1738,7 +1748,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
@@ -1746,7 +1756,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
@@ -1754,7 +1764,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13">
       <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
@@ -1762,7 +1772,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="A14" s="1" t="s">
         <v>58</v>
       </c>
@@ -1770,7 +1780,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15">
       <c r="A15" s="1" t="s">
         <v>63</v>
       </c>
@@ -1778,7 +1788,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16">
       <c r="A16" s="1" t="s">
         <v>74</v>
       </c>
@@ -1786,7 +1796,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17">
       <c r="A17" s="1" t="s">
         <v>91</v>
       </c>
@@ -1795,23 +1805,22 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>107</v>
       </c>
@@ -1819,7 +1828,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" s="1" t="s">
         <v>82</v>
       </c>
@@ -1827,7 +1836,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" s="1" t="s">
         <v>44</v>
       </c>
@@ -1835,7 +1844,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -1843,43 +1852,43 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="A5" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6">
       <c r="A6" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7">
       <c r="A7" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8">
       <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9">
       <c r="A9" s="1" t="s">
         <v>65</v>
       </c>
@@ -1887,7 +1896,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
@@ -1895,7 +1904,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="A11" s="1" t="s">
         <v>70</v>
       </c>
@@ -1903,7 +1912,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="A12" s="1" t="s">
         <v>85</v>
       </c>
@@ -1911,7 +1920,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13">
       <c r="A13" s="1" t="s">
         <v>60</v>
       </c>
@@ -1919,7 +1928,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -1927,7 +1936,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15">
       <c r="A15" s="1" t="s">
         <v>75</v>
       </c>
@@ -1935,7 +1944,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16">
       <c r="A16" s="1" t="s">
         <v>51</v>
       </c>
@@ -1943,7 +1952,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17">
       <c r="A17" s="1" t="s">
         <v>90</v>
       </c>
@@ -1952,23 +1961,22 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>107</v>
       </c>
@@ -1976,7 +1984,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" s="1" t="s">
         <v>43</v>
       </c>
@@ -1984,7 +1992,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" s="1" t="s">
         <v>84</v>
       </c>
@@ -1992,7 +2000,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" s="1" t="s">
         <v>33</v>
       </c>
@@ -2000,7 +2008,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="A5" s="1" t="s">
         <v>59</v>
       </c>
@@ -2008,7 +2016,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="A6" s="1" t="s">
         <v>62</v>
       </c>
@@ -2016,7 +2024,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="A7" s="1" t="s">
         <v>77</v>
       </c>
@@ -2024,7 +2032,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -2032,7 +2040,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="A9" s="1" t="s">
         <v>52</v>
       </c>
@@ -2040,7 +2048,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10">
       <c r="A10" s="1" t="s">
         <v>69</v>
       </c>
@@ -2048,34 +2056,34 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="A11" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="I11" s="4"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12">
       <c r="A12" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14">
       <c r="A14" s="1" t="s">
         <v>37</v>
       </c>
@@ -2083,7 +2091,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15">
       <c r="A15" s="1" t="s">
         <v>51</v>
       </c>
@@ -2091,7 +2099,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16">
       <c r="A16" s="1" t="s">
         <v>91</v>
       </c>
@@ -2099,7 +2107,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17">
       <c r="A17" s="1" t="s">
         <v>88</v>
       </c>
@@ -2108,23 +2116,22 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>107</v>
       </c>
@@ -2132,7 +2139,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" s="1" t="s">
         <v>44</v>
       </c>
@@ -2140,52 +2147,52 @@
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4">
       <c r="A4" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5">
       <c r="A5" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6">
       <c r="A6" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7">
       <c r="A7" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -2193,7 +2200,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="A9" s="1" t="s">
         <v>91</v>
       </c>
@@ -2201,7 +2208,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10">
       <c r="A10" s="1" t="s">
         <v>82</v>
       </c>
@@ -2209,7 +2216,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="A11" s="1" t="s">
         <v>32</v>
       </c>
@@ -2217,7 +2224,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="A12" s="1" t="s">
         <v>71</v>
       </c>
@@ -2225,7 +2232,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13">
       <c r="A13" s="1" t="s">
         <v>60</v>
       </c>
@@ -2233,7 +2240,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
@@ -2241,7 +2248,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15">
       <c r="A15" s="1" t="s">
         <v>37</v>
       </c>
@@ -2249,7 +2256,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16">
       <c r="A16" s="1" t="s">
         <v>77</v>
       </c>
@@ -2257,7 +2264,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17">
       <c r="A17" s="1" t="s">
         <v>52</v>
       </c>
@@ -2266,157 +2273,308 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F10" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E11" s="1" t="s">
@@ -2426,135 +2584,134 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="3" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F97"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2562,7 +2719,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -2570,7 +2727,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -2580,7 +2737,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -2590,7 +2747,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -2600,7 +2757,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -2610,7 +2767,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -2620,7 +2777,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -2630,7 +2787,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -2640,7 +2797,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -2650,7 +2807,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -2658,7 +2815,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -2666,7 +2823,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -2674,7 +2831,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -2682,7 +2839,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -2690,7 +2847,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -2698,7 +2855,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -2706,7 +2863,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
@@ -2714,7 +2871,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
@@ -2722,7 +2879,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
@@ -2730,7 +2887,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -2738,7 +2895,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
@@ -2746,7 +2903,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -2754,7 +2911,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
@@ -2762,7 +2919,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
@@ -2770,7 +2927,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26">
       <c r="A26" s="1" t="s">
         <v>28</v>
       </c>
@@ -2778,7 +2935,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27">
       <c r="A27" s="1" t="s">
         <v>30</v>
       </c>
@@ -2786,7 +2943,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28">
       <c r="A28" s="1" t="s">
         <v>31</v>
       </c>
@@ -2794,7 +2951,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29">
       <c r="A29" s="1" t="s">
         <v>32</v>
       </c>
@@ -2802,7 +2959,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30">
       <c r="A30" s="1" t="s">
         <v>33</v>
       </c>
@@ -2810,7 +2967,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31">
       <c r="A31" s="1" t="s">
         <v>34</v>
       </c>
@@ -2818,7 +2975,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32">
       <c r="A32" s="1" t="s">
         <v>35</v>
       </c>
@@ -2826,7 +2983,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33">
       <c r="A33" s="1" t="s">
         <v>36</v>
       </c>
@@ -2834,7 +2991,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34">
       <c r="A34" s="1" t="s">
         <v>37</v>
       </c>
@@ -2842,7 +2999,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35">
       <c r="A35" s="1" t="s">
         <v>38</v>
       </c>
@@ -2850,7 +3007,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36">
       <c r="A36" s="1" t="s">
         <v>39</v>
       </c>
@@ -2858,7 +3015,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37">
       <c r="A37" s="1" t="s">
         <v>40</v>
       </c>
@@ -2866,7 +3023,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38">
       <c r="A38" s="1" t="s">
         <v>41</v>
       </c>
@@ -2874,7 +3031,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39">
       <c r="A39" s="1" t="s">
         <v>43</v>
       </c>
@@ -2882,7 +3039,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40">
       <c r="A40" s="1" t="s">
         <v>44</v>
       </c>
@@ -2890,7 +3047,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41">
       <c r="A41" s="1" t="s">
         <v>45</v>
       </c>
@@ -2898,7 +3055,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42">
       <c r="A42" s="1" t="s">
         <v>46</v>
       </c>
@@ -2906,7 +3063,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43">
       <c r="A43" s="1" t="s">
         <v>47</v>
       </c>
@@ -2914,7 +3071,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44">
       <c r="A44" s="1" t="s">
         <v>48</v>
       </c>
@@ -2922,7 +3079,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45">
       <c r="A45" s="1" t="s">
         <v>49</v>
       </c>
@@ -2930,7 +3087,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46">
       <c r="A46" s="1" t="s">
         <v>50</v>
       </c>
@@ -2938,7 +3095,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47">
       <c r="A47" s="1" t="s">
         <v>51</v>
       </c>
@@ -2946,7 +3103,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48">
       <c r="A48" s="1" t="s">
         <v>52</v>
       </c>
@@ -2954,7 +3111,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49">
       <c r="A49" s="1" t="s">
         <v>53</v>
       </c>
@@ -2962,7 +3119,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50">
       <c r="A50" s="1" t="s">
         <v>54</v>
       </c>
@@ -2970,7 +3127,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51">
       <c r="A51" s="1" t="s">
         <v>56</v>
       </c>
@@ -2978,7 +3135,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52">
       <c r="A52" s="1" t="s">
         <v>57</v>
       </c>
@@ -2986,7 +3143,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53">
       <c r="A53" s="1" t="s">
         <v>58</v>
       </c>
@@ -2994,7 +3151,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54">
       <c r="A54" s="1" t="s">
         <v>59</v>
       </c>
@@ -3002,7 +3159,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55">
       <c r="A55" s="1" t="s">
         <v>60</v>
       </c>
@@ -3010,7 +3167,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56">
       <c r="A56" s="1" t="s">
         <v>61</v>
       </c>
@@ -3018,7 +3175,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57">
       <c r="A57" s="1" t="s">
         <v>62</v>
       </c>
@@ -3026,7 +3183,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="58">
       <c r="A58" s="1" t="s">
         <v>63</v>
       </c>
@@ -3034,7 +3191,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59">
       <c r="A59" s="1" t="s">
         <v>64</v>
       </c>
@@ -3042,7 +3199,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60">
       <c r="A60" s="1" t="s">
         <v>65</v>
       </c>
@@ -3050,7 +3207,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="61">
       <c r="A61" s="1" t="s">
         <v>66</v>
       </c>
@@ -3058,7 +3215,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="62">
       <c r="A62" s="1" t="s">
         <v>67</v>
       </c>
@@ -3066,7 +3223,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="63">
       <c r="A63" s="1" t="s">
         <v>69</v>
       </c>
@@ -3074,7 +3231,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="64">
       <c r="A64" s="1" t="s">
         <v>70</v>
       </c>
@@ -3082,7 +3239,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="65">
       <c r="A65" s="1" t="s">
         <v>71</v>
       </c>
@@ -3090,7 +3247,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="66">
       <c r="A66" s="1" t="s">
         <v>72</v>
       </c>
@@ -3098,7 +3255,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="67">
       <c r="A67" s="1" t="s">
         <v>73</v>
       </c>
@@ -3106,7 +3263,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="68">
       <c r="A68" s="1" t="s">
         <v>74</v>
       </c>
@@ -3114,7 +3271,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="69">
       <c r="A69" s="1" t="s">
         <v>75</v>
       </c>
@@ -3122,7 +3279,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="70">
       <c r="A70" s="1" t="s">
         <v>76</v>
       </c>
@@ -3130,7 +3287,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="71">
       <c r="A71" s="1" t="s">
         <v>77</v>
       </c>
@@ -3138,7 +3295,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="72">
       <c r="A72" s="1" t="s">
         <v>78</v>
       </c>
@@ -3146,7 +3303,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="73">
       <c r="A73" s="1" t="s">
         <v>79</v>
       </c>
@@ -3154,7 +3311,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="74">
       <c r="A74" s="1" t="s">
         <v>80</v>
       </c>
@@ -3162,7 +3319,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="75">
       <c r="A75" s="1" t="s">
         <v>82</v>
       </c>
@@ -3170,7 +3327,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="76">
       <c r="A76" s="1" t="s">
         <v>83</v>
       </c>
@@ -3178,7 +3335,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="77">
       <c r="A77" s="1" t="s">
         <v>84</v>
       </c>
@@ -3186,7 +3343,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="78">
       <c r="A78" s="1" t="s">
         <v>85</v>
       </c>
@@ -3194,7 +3351,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="79">
       <c r="A79" s="1" t="s">
         <v>86</v>
       </c>
@@ -3202,7 +3359,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="80">
       <c r="A80" s="1" t="s">
         <v>87</v>
       </c>
@@ -3210,7 +3367,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81">
       <c r="A81" s="1" t="s">
         <v>88</v>
       </c>
@@ -3218,7 +3375,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="82">
       <c r="A82" s="1" t="s">
         <v>89</v>
       </c>
@@ -3226,7 +3383,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="83">
       <c r="A83" s="1" t="s">
         <v>90</v>
       </c>
@@ -3234,7 +3391,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="84">
       <c r="A84" s="1" t="s">
         <v>91</v>
       </c>
@@ -3242,7 +3399,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="85">
       <c r="A85" s="1" t="s">
         <v>92</v>
       </c>
@@ -3250,7 +3407,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="86">
       <c r="A86" s="1" t="s">
         <v>93</v>
       </c>
@@ -3258,7 +3415,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="87">
       <c r="A87" s="1" t="s">
         <v>95</v>
       </c>
@@ -3266,7 +3423,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="88">
       <c r="A88" s="1" t="s">
         <v>96</v>
       </c>
@@ -3274,7 +3431,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="89">
       <c r="A89" s="1" t="s">
         <v>97</v>
       </c>
@@ -3282,7 +3439,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="90">
       <c r="A90" s="1" t="s">
         <v>99</v>
       </c>
@@ -3290,7 +3447,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="91">
       <c r="A91" s="1" t="s">
         <v>100</v>
       </c>
@@ -3298,7 +3455,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="92">
       <c r="A92" s="1" t="s">
         <v>101</v>
       </c>
@@ -3306,7 +3463,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="93">
       <c r="A93" s="1" t="s">
         <v>102</v>
       </c>
@@ -3314,7 +3471,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="94">
       <c r="A94" s="1" t="s">
         <v>103</v>
       </c>
@@ -3322,7 +3479,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="95">
       <c r="A95" s="1" t="s">
         <v>104</v>
       </c>
@@ -3330,7 +3487,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="96">
       <c r="A96" s="1" t="s">
         <v>105</v>
       </c>
@@ -3338,7 +3495,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97">
       <c r="A97" s="1" t="s">
         <v>106</v>
       </c>
@@ -3347,22 +3504,21 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3370,7 +3526,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -3378,7 +3534,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -3386,7 +3542,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -3394,7 +3550,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -3402,7 +3558,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -3410,7 +3566,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -3418,7 +3574,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -3426,7 +3582,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -3434,7 +3590,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -3442,7 +3598,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -3450,7 +3606,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -3458,7 +3614,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -3466,7 +3622,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -3474,7 +3630,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -3482,7 +3638,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -3490,7 +3646,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -3498,7 +3654,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
@@ -3506,7 +3662,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
@@ -3514,7 +3670,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
@@ -3522,7 +3678,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -3530,7 +3686,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
@@ -3538,7 +3694,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -3546,7 +3702,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
@@ -3554,7 +3710,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
@@ -3563,22 +3719,21 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3586,7 +3741,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -3594,7 +3749,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -3602,7 +3757,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -3610,7 +3765,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -3618,7 +3773,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -3626,7 +3781,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -3634,7 +3789,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -3642,7 +3797,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -3650,7 +3805,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -3658,7 +3813,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -3666,7 +3821,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -3674,7 +3829,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -3682,7 +3837,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -3690,7 +3845,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -3698,7 +3853,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -3706,7 +3861,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -3714,7 +3869,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
@@ -3722,7 +3877,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
@@ -3730,7 +3885,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
@@ -3738,7 +3893,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -3746,7 +3901,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
@@ -3754,7 +3909,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -3762,7 +3917,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
@@ -3770,7 +3925,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
@@ -3779,22 +3934,21 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3802,7 +3956,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -3810,7 +3964,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -3818,7 +3972,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -3826,7 +3980,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -3834,7 +3988,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -3842,7 +3996,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -3850,7 +4004,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -3858,7 +4012,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -3866,7 +4020,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -3874,7 +4028,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -3882,7 +4036,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -3890,7 +4044,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -3898,7 +4052,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -3906,7 +4060,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -3914,7 +4068,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -3922,7 +4076,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -3930,7 +4084,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
@@ -3938,7 +4092,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
@@ -3946,7 +4100,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
@@ -3954,7 +4108,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -3962,7 +4116,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
@@ -3970,7 +4124,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -3978,7 +4132,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
@@ -3986,7 +4140,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
@@ -3995,22 +4149,21 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>107</v>
       </c>
@@ -4018,7 +4171,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" s="1" t="s">
         <v>82</v>
       </c>
@@ -4026,7 +4179,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
@@ -4034,16 +4187,16 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5">
       <c r="A5" s="1" t="s">
         <v>60</v>
       </c>
@@ -4051,34 +4204,34 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="A6" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7">
       <c r="A7" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9">
       <c r="A9" s="1" t="s">
         <v>78</v>
       </c>
@@ -4086,7 +4239,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
@@ -4094,7 +4247,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="A11" s="1" t="s">
         <v>70</v>
       </c>
@@ -4102,7 +4255,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="A12" s="1" t="s">
         <v>45</v>
       </c>
@@ -4110,7 +4263,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13">
       <c r="A13" s="1" t="s">
         <v>85</v>
       </c>
@@ -4118,7 +4271,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -4126,7 +4279,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15">
       <c r="A15" s="1" t="s">
         <v>63</v>
       </c>
@@ -4134,7 +4287,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16">
       <c r="A16" s="1" t="s">
         <v>89</v>
       </c>
@@ -4142,7 +4295,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17">
       <c r="A17" s="1" t="s">
         <v>38</v>
       </c>
@@ -4151,23 +4304,22 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>107</v>
       </c>
@@ -4175,7 +4327,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -4183,7 +4335,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -4191,7 +4343,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" s="1" t="s">
         <v>31</v>
       </c>
@@ -4199,7 +4351,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="A5" s="1" t="s">
         <v>49</v>
       </c>
@@ -4207,7 +4359,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="A6" s="1" t="s">
         <v>60</v>
       </c>
@@ -4215,7 +4367,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="A7" s="1" t="s">
         <v>78</v>
       </c>
@@ -4223,7 +4375,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="A8" s="1" t="s">
         <v>82</v>
       </c>
@@ -4231,7 +4383,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="A9" s="1" t="s">
         <v>87</v>
       </c>
@@ -4240,22 +4392,21 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>107</v>
       </c>
@@ -4263,7 +4414,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -4271,7 +4422,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" s="1" t="s">
         <v>43</v>
       </c>
@@ -4279,7 +4430,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" s="1" t="s">
         <v>48</v>
       </c>
@@ -4287,7 +4438,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="A5" s="1" t="s">
         <v>50</v>
       </c>
@@ -4295,34 +4446,34 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="A6" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7">
       <c r="A7" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8">
       <c r="A8" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9">
       <c r="A9" s="1" t="s">
         <v>91</v>
       </c>
@@ -4330,7 +4481,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -4338,7 +4489,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -4346,7 +4497,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="A12" s="1" t="s">
         <v>31</v>
       </c>
@@ -4354,7 +4505,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13">
       <c r="A13" s="1" t="s">
         <v>52</v>
       </c>
@@ -4362,7 +4513,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="A14" s="1" t="s">
         <v>60</v>
       </c>
@@ -4370,7 +4521,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15">
       <c r="A15" s="1" t="s">
         <v>69</v>
       </c>
@@ -4378,7 +4529,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16">
       <c r="A16" s="1" t="s">
         <v>76</v>
       </c>
@@ -4386,7 +4537,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17">
       <c r="A17" s="1" t="s">
         <v>85</v>
       </c>
@@ -4395,7 +4546,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added 41 deg 48 hr
</commit_message>
<xml_diff>
--- a/data-raw/Growth curve well labels.xlsx
+++ b/data-raw/Growth curve well labels.xlsx
@@ -17,6 +17,7 @@
     <sheet state="visible" name="06.07, 40.5 deg" sheetId="12" r:id="rId15"/>
     <sheet state="visible" name="11.07, 41 deg" sheetId="13" r:id="rId16"/>
     <sheet state="visible" name="14.07, 30 deg" sheetId="14" r:id="rId17"/>
+    <sheet state="visible" name="13.07, 41 deg, 48 hr" sheetId="15" r:id="rId18"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -153,7 +154,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="123">
   <si>
     <t xml:space="preserve">well </t>
   </si>
@@ -619,6 +620,10 @@
 </file>
 
 <file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -2435,6 +2440,157 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
added well key for july 17 42 deg 72 hr
</commit_message>
<xml_diff>
--- a/data-raw/Growth curve well labels.xlsx
+++ b/data-raw/Growth curve well labels.xlsx
@@ -4,20 +4,21 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="16.06, 20.06" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="joey-edit-16.06, 20.06" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="24.06" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="28.06, 30 and 34 deg" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="29.06, 37 deg" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="30.06, 40 and 41 deg" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="01.07, 25 deg" sheetId="7" r:id="rId10"/>
-    <sheet state="visible" name="04.07, 18 deg" sheetId="8" r:id="rId11"/>
-    <sheet state="visible" name="05.07, 30 deg" sheetId="9" r:id="rId12"/>
-    <sheet state="visible" name="05.07, 40 deg" sheetId="10" r:id="rId13"/>
-    <sheet state="visible" name="06.07, 37 deg" sheetId="11" r:id="rId14"/>
-    <sheet state="visible" name="06.07, 40.5 deg" sheetId="12" r:id="rId15"/>
-    <sheet state="visible" name="11.07, 41 deg" sheetId="13" r:id="rId16"/>
-    <sheet state="visible" name="14.07, 30 deg" sheetId="14" r:id="rId17"/>
-    <sheet state="visible" name="13.07, 41 deg, 48 hr" sheetId="15" r:id="rId18"/>
+    <sheet state="visible" name="17.07, 42 deg, 72 hr" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="joey-edit-16.06, 20.06" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="24.06" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="28.06, 30 and 34 deg" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="29.06, 37 deg" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="30.06, 40 and 41 deg" sheetId="7" r:id="rId10"/>
+    <sheet state="visible" name="01.07, 25 deg" sheetId="8" r:id="rId11"/>
+    <sheet state="visible" name="04.07, 18 deg" sheetId="9" r:id="rId12"/>
+    <sheet state="visible" name="05.07, 30 deg" sheetId="10" r:id="rId13"/>
+    <sheet state="visible" name="05.07, 40 deg" sheetId="11" r:id="rId14"/>
+    <sheet state="visible" name="06.07, 37 deg" sheetId="12" r:id="rId15"/>
+    <sheet state="visible" name="06.07, 40.5 deg" sheetId="13" r:id="rId16"/>
+    <sheet state="visible" name="11.07, 41 deg" sheetId="14" r:id="rId17"/>
+    <sheet state="visible" name="14.07, 30 deg" sheetId="15" r:id="rId18"/>
+    <sheet state="visible" name="13.07, 41 deg, 48 hr" sheetId="16" r:id="rId19"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -154,7 +155,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="123">
   <si>
     <t xml:space="preserve">well </t>
   </si>
@@ -477,6 +478,12 @@
     <t>H12</t>
   </si>
   <si>
+    <t>treatment</t>
+  </si>
+  <si>
+    <t>fRS585</t>
+  </si>
+  <si>
     <t>well</t>
   </si>
   <si>
@@ -505,12 +512,6 @@
   </si>
   <si>
     <t>H 4-12</t>
-  </si>
-  <si>
-    <t>treatment</t>
-  </si>
-  <si>
-    <t>fRS585</t>
   </si>
   <si>
     <t>fRS1</t>
@@ -624,6 +625,10 @@
 </file>
 
 <file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing16.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1672,82 +1677,82 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E6" s="4"/>
+        <v>108</v>
+      </c>
+      <c r="D6" s="4"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E7" s="4"/>
+        <v>108</v>
+      </c>
+      <c r="D7" s="4"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E8" s="4"/>
+        <v>108</v>
+      </c>
+      <c r="D8" s="4"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>94</v>
@@ -1755,7 +1760,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>94</v>
@@ -1763,7 +1768,7 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>94</v>
@@ -1771,7 +1776,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>94</v>
@@ -1779,7 +1784,7 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>94</v>
@@ -1787,7 +1792,7 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>94</v>
@@ -1795,7 +1800,7 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>94</v>
@@ -1803,7 +1808,7 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>94</v>
@@ -1827,83 +1832,82 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>82</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E5" s="5"/>
+        <v>108</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="E6" s="4"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="E7" s="4"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>84</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E8" s="6"/>
+        <v>108</v>
+      </c>
+      <c r="E8" s="4"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>94</v>
@@ -1911,7 +1915,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>70</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>94</v>
@@ -1919,7 +1923,7 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>85</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>94</v>
@@ -1927,7 +1931,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>94</v>
@@ -1935,7 +1939,7 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>94</v>
@@ -1943,7 +1947,7 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>94</v>
@@ -1951,7 +1955,7 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>94</v>
@@ -1959,7 +1963,7 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>94</v>
@@ -1983,79 +1987,83 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>43</v>
+        <v>82</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>118</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="E5" s="5"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>62</v>
+        <v>87</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>118</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="E6" s="4"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>77</v>
+        <v>37</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>118</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="E7" s="4"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>118</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="E8" s="6"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>69</v>
+        <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>94</v>
@@ -2063,34 +2071,31 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="I11" s="5"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="I12" s="4"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="I13" s="4"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>94</v>
@@ -2098,7 +2103,7 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>94</v>
@@ -2106,7 +2111,7 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>91</v>
+        <v>51</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>94</v>
@@ -2114,7 +2119,7 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>94</v>
@@ -2138,84 +2143,79 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D3" s="4"/>
+        <v>108</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D4" s="5"/>
+        <v>108</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D5" s="4"/>
+        <v>108</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D6" s="4"/>
+        <v>108</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D7" s="6"/>
+        <v>108</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>91</v>
+        <v>52</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>94</v>
@@ -2223,31 +2223,34 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>94</v>
       </c>
+      <c r="I11" s="5"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>94</v>
       </c>
+      <c r="I12" s="4"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>94</v>
       </c>
+      <c r="I13" s="4"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>94</v>
@@ -2255,7 +2258,7 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>94</v>
@@ -2263,7 +2266,7 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>94</v>
@@ -2271,7 +2274,7 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>52</v>
+        <v>88</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>94</v>
@@ -2295,127 +2298,127 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>70</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C3" s="4"/>
+        <v>108</v>
+      </c>
+      <c r="D3" s="4"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C4" s="4"/>
+        <v>108</v>
+      </c>
+      <c r="D4" s="5"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>47</v>
+        <v>87</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C5" s="6"/>
+        <v>108</v>
+      </c>
+      <c r="D5" s="4"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>118</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="D6" s="4"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D7" s="4"/>
+        <v>108</v>
+      </c>
+      <c r="D7" s="6"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>89</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D8" s="6"/>
+        <v>108</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>38</v>
+        <v>91</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>31</v>
+        <v>82</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>84</v>
+        <v>32</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>71</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16">
@@ -2423,7 +2426,7 @@
         <v>77</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17">
@@ -2431,7 +2434,7 @@
         <v>52</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2452,10 +2455,167 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>107</v>
       </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2">
@@ -2463,7 +2623,7 @@
         <v>44</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3">
@@ -2471,7 +2631,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4">
@@ -2479,7 +2639,7 @@
         <v>84</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5">
@@ -2487,7 +2647,7 @@
         <v>87</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6">
@@ -2495,7 +2655,7 @@
         <v>49</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7">
@@ -2503,7 +2663,7 @@
         <v>76</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8">
@@ -2511,7 +2671,7 @@
         <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9">
@@ -2519,7 +2679,7 @@
         <v>91</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10">
@@ -2603,253 +2763,146 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>3</v>
+        <v>19</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>3</v>
+        <v>25</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>29</v>
+        <v>49</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>42</v>
+        <v>71</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>55</v>
+        <v>76</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>68</v>
+        <v>84</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>81</v>
+        <v>87</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>98</v>
+        <v>22</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>3</v>
+        <v>32</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>3</v>
+        <v>37</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>16</v>
+        <v>52</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>16</v>
+        <v>60</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>16</v>
+        <v>77</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>16</v>
+        <v>82</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>16</v>
+        <v>71</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2869,794 +2922,253 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>118</v>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="B5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="B6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="B7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="B8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="B9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="B10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>118</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>118</v>
+      <c r="B12" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>118</v>
+      <c r="B13" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>119</v>
+      <c r="B14" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>119</v>
+      <c r="B15" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>119</v>
+      <c r="B16" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>119</v>
+      <c r="B17" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>119</v>
+      <c r="B18" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>119</v>
+      <c r="B19" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>119</v>
+      <c r="B20" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>119</v>
+      <c r="B21" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>119</v>
+      <c r="B22" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>119</v>
+      <c r="B23" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>119</v>
+      <c r="B24" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>98</v>
+      <c r="B25" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -3679,199 +3191,791 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>118</v>
+      <c r="B2" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>118</v>
-      </c>
+      <c r="B3" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>118</v>
-      </c>
+      <c r="B4" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>118</v>
-      </c>
+      <c r="B5" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>118</v>
-      </c>
+      <c r="B6" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>118</v>
-      </c>
+      <c r="B7" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>118</v>
-      </c>
+      <c r="B8" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>118</v>
-      </c>
+      <c r="B9" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>118</v>
-      </c>
+      <c r="B10" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>118</v>
+      <c r="B11" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>118</v>
+      <c r="B12" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>118</v>
+      <c r="B13" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>94</v>
+      <c r="B14" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>94</v>
+      <c r="B15" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>94</v>
+      <c r="B16" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>94</v>
+      <c r="B17" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>94</v>
+      <c r="B18" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>94</v>
+      <c r="B19" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>94</v>
+      <c r="B20" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>94</v>
+      <c r="B21" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>94</v>
+      <c r="B22" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>94</v>
+      <c r="B23" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>94</v>
+      <c r="B24" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>94</v>
+      <c r="B25" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -3894,7 +3998,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2">
@@ -3902,7 +4006,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3">
@@ -3910,7 +4014,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4">
@@ -3918,7 +4022,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5">
@@ -3926,7 +4030,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6">
@@ -3934,7 +4038,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7">
@@ -3942,7 +4046,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8">
@@ -3950,7 +4054,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9">
@@ -3958,7 +4062,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10">
@@ -3966,7 +4070,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11">
@@ -3974,7 +4078,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12">
@@ -3982,7 +4086,7 @@
         <v>13</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13">
@@ -3990,7 +4094,7 @@
         <v>14</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14">
@@ -4109,7 +4213,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2">
@@ -4117,7 +4221,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3">
@@ -4125,7 +4229,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4">
@@ -4133,7 +4237,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5">
@@ -4141,7 +4245,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6">
@@ -4149,7 +4253,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7">
@@ -4157,7 +4261,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8">
@@ -4165,7 +4269,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9">
@@ -4173,7 +4277,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10">
@@ -4181,7 +4285,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11">
@@ -4189,7 +4293,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12">
@@ -4197,7 +4301,7 @@
         <v>13</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13">
@@ -4205,7 +4309,7 @@
         <v>14</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14">
@@ -4321,115 +4425,111 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>82</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D4" s="4"/>
+        <v>108</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>87</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D6" s="5"/>
+        <v>108</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D7" s="4"/>
+        <v>108</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D8" s="4"/>
+        <v>108</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>78</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>94</v>
@@ -4437,7 +4537,7 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>94</v>
@@ -4445,7 +4545,7 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>89</v>
+        <v>18</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>94</v>
@@ -4453,15 +4553,78 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>94</v>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
   </sheetData>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4477,78 +4640,147 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>82</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>118</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="D4" s="4"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>118</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="D6" s="5"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>118</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="D7" s="4"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>82</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>118</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="D8" s="4"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -4564,10 +4796,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="2">
@@ -4575,134 +4807,66 @@
         <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D6" s="4"/>
+        <v>108</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D7" s="4"/>
+        <v>108</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D8" s="4"/>
+        <v>108</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>